<commit_message>
EPBDS-10212 @class appears in REST response
</commit_message>
<xml_diff>
--- a/ITEST/itest.jacksonbinding/openl-repository/deployments/smartdefaulttyping/smartdefaulttyping.xlsx
+++ b/ITEST/itest.jacksonbinding/openl-repository/deployments/smartdefaulttyping/smartdefaulttyping.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.jacksonbinding\openl-repository\deployments\smartdefaulttyping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DCA704-2F9A-4168-BE59-3F9BDD233841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>String</t>
   </si>
@@ -116,12 +122,18 @@
   </si>
   <si>
     <t>Method Dog myDog()</t>
+  </si>
+  <si>
+    <t>smart</t>
+  </si>
+  <si>
+    <t>Datatype HomeCat extends Cat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -158,7 +170,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -185,7 +197,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -193,6 +205,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -545,36 +560,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.81640625" style="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -591,7 +606,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -602,7 +617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -611,7 +626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -622,7 +637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -630,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -639,7 +654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -650,7 +665,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
@@ -660,7 +675,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
@@ -674,7 +689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
@@ -688,7 +703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
@@ -702,7 +717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
@@ -716,13 +731,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
@@ -730,7 +745,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
@@ -738,15 +753,30 @@
         <v>28</v>
       </c>
     </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>